<commit_message>
Adding the IPA changes
</commit_message>
<xml_diff>
--- a/src/test/test-data/IPA.xlsx
+++ b/src/test/test-data/IPA.xlsx
@@ -4,25 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Competetitors" sheetId="1" r:id="rId1"/>
     <sheet name="Dashboard" sheetId="2" r:id="rId2"/>
     <sheet name="Filters" sheetId="3" r:id="rId3"/>
     <sheet name="Resultset" sheetId="4" r:id="rId4"/>
-    <sheet name="Search" sheetId="5" r:id="rId5"/>
-    <sheet name="Snapshot" sheetId="6" r:id="rId6"/>
-    <sheet name="Techprofolio" sheetId="7" r:id="rId7"/>
-    <sheet name="Techtrending" sheetId="8" r:id="rId8"/>
-    <sheet name="Visual" sheetId="9" r:id="rId9"/>
+    <sheet name="Snapshot" sheetId="6" r:id="rId5"/>
+    <sheet name="Techprofolio" sheetId="7" r:id="rId6"/>
+    <sheet name="Techtrending" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="67">
   <si>
     <t>GET</t>
   </si>
@@ -180,18 +178,6 @@
     <t>resultset-company</t>
   </si>
   <si>
-    <t>SEARCH</t>
-  </si>
-  <si>
-    <t>API Test for search</t>
-  </si>
-  <si>
-    <t>/analytics/search</t>
-  </si>
-  <si>
-    <t>?query=laser</t>
-  </si>
-  <si>
     <t>snapshot-technology</t>
   </si>
   <si>
@@ -235,15 +221,6 @@
   </si>
   <si>
     <t>API Test for techtrending for company search</t>
-  </si>
-  <si>
-    <t>visual</t>
-  </si>
-  <si>
-    <t>API Test for visuals</t>
-  </si>
-  <si>
-    <t>/analytics/visual</t>
   </si>
 </sst>
 </file>
@@ -3083,526 +3060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="53.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="49.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="52.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="96.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="5" width="80.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="5" width="90.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75">
-      <c r="A2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="L2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75">
-      <c r="A3" s="8"/>
-      <c r="B3" s="11"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-    </row>
-    <row r="4" spans="1:12" s="18" customFormat="1" ht="15.75">
-      <c r="A4" s="16"/>
-      <c r="B4" s="17"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4" s="19"/>
-      <c r="I4"/>
-      <c r="J4" s="19"/>
-      <c r="K4"/>
-      <c r="L4"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.75">
-      <c r="A5" s="8"/>
-      <c r="B5" s="11"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5" s="5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.75">
-      <c r="A6" s="8"/>
-      <c r="B6" s="11"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6" s="5"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.75">
-      <c r="A7" s="8"/>
-      <c r="B7" s="11"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7" s="5"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-    </row>
-    <row r="8" spans="1:12" ht="15.75">
-      <c r="A8" s="8"/>
-      <c r="B8" s="11"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8" s="1"/>
-      <c r="F8"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="1"/>
-      <c r="L8"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="8"/>
-      <c r="B9" s="13"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9" s="7"/>
-      <c r="I9"/>
-      <c r="J9" s="4"/>
-      <c r="K9"/>
-      <c r="L9"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.75">
-      <c r="A10" s="8"/>
-      <c r="B10" s="11"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10" s="7"/>
-      <c r="I10"/>
-      <c r="J10"/>
-      <c r="K10"/>
-      <c r="L10"/>
-    </row>
-    <row r="11" spans="1:12" ht="16.5">
-      <c r="A11" s="8"/>
-      <c r="B11" s="11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="8"/>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11"/>
-    </row>
-    <row r="12" spans="1:12" ht="16.5">
-      <c r="A12" s="8"/>
-      <c r="B12" s="11"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="8"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-    </row>
-    <row r="13" spans="1:12" ht="16.5">
-      <c r="A13" s="8"/>
-      <c r="B13" s="11"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="8"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75">
-      <c r="A14" s="8"/>
-      <c r="B14" s="11"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14" s="7"/>
-      <c r="I14"/>
-      <c r="J14"/>
-      <c r="K14"/>
-      <c r="L14"/>
-    </row>
-    <row r="15" spans="1:12" ht="16.5">
-      <c r="A15" s="8"/>
-      <c r="B15" s="11"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="8"/>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.75">
-      <c r="A16" s="8"/>
-      <c r="B16" s="14"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.75">
-      <c r="A17" s="8"/>
-      <c r="B17" s="12"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17"/>
-      <c r="K17"/>
-      <c r="L17"/>
-    </row>
-    <row r="18" spans="1:12" ht="15.75">
-      <c r="A18" s="8"/>
-      <c r="B18" s="11"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18" s="1"/>
-      <c r="F18"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="1"/>
-      <c r="L18"/>
-    </row>
-    <row r="19" spans="1:12" ht="15.75">
-      <c r="A19" s="8"/>
-      <c r="B19" s="11"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19" s="1"/>
-      <c r="F19"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="1"/>
-      <c r="L19"/>
-    </row>
-    <row r="20" spans="1:12" ht="15.75">
-      <c r="A20" s="8"/>
-      <c r="B20" s="11"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20" s="1"/>
-      <c r="F20"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="1"/>
-      <c r="L20"/>
-    </row>
-    <row r="21" spans="1:12" s="9" customFormat="1" ht="15.75">
-      <c r="A21" s="8"/>
-      <c r="B21" s="15"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21" s="8"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21" s="10"/>
-      <c r="I21"/>
-      <c r="J21" s="13"/>
-      <c r="K21"/>
-      <c r="L21"/>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22" s="8"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-      <c r="J22" s="4"/>
-      <c r="K22"/>
-      <c r="L22"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23" s="8"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23" s="4"/>
-      <c r="I23"/>
-      <c r="J23" s="4"/>
-      <c r="K23"/>
-      <c r="L23"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24" s="8"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
-      <c r="J24" s="4"/>
-      <c r="K24"/>
-      <c r="L24"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25"/>
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25" s="1"/>
-      <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25"/>
-      <c r="I25"/>
-      <c r="J25"/>
-      <c r="K25"/>
-      <c r="L25"/>
-    </row>
-    <row r="26" spans="1:12" ht="15.75">
-      <c r="A26"/>
-      <c r="B26" s="11"/>
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="4"/>
-      <c r="K26"/>
-      <c r="L26"/>
-    </row>
-    <row r="27" spans="1:12" ht="15.75">
-      <c r="A27"/>
-      <c r="B27" s="11"/>
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="7"/>
-      <c r="K27"/>
-      <c r="L27"/>
-    </row>
-    <row r="28" spans="1:12" ht="15.75">
-      <c r="A28"/>
-      <c r="B28" s="11"/>
-      <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="4"/>
-      <c r="K28"/>
-      <c r="L28"/>
-    </row>
-    <row r="29" spans="1:12" ht="15.75">
-      <c r="A29"/>
-      <c r="B29" s="11"/>
-      <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29" s="1"/>
-      <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="4"/>
-      <c r="K29"/>
-      <c r="L29"/>
-    </row>
-    <row r="30" spans="1:12" ht="15.75">
-      <c r="A30"/>
-      <c r="B30" s="11"/>
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30" s="1"/>
-      <c r="F30"/>
-      <c r="G30"/>
-      <c r="H30"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="4"/>
-      <c r="K30"/>
-      <c r="L30"/>
-    </row>
-    <row r="31" spans="1:12" ht="15.75">
-      <c r="A31"/>
-      <c r="B31" s="11"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="4"/>
-      <c r="K31"/>
-      <c r="L31"/>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="8"/>
-      <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32" s="8"/>
-      <c r="F32"/>
-      <c r="G32"/>
-      <c r="H32"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="4"/>
-      <c r="K32"/>
-      <c r="L32"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -3662,16 +3120,16 @@
     </row>
     <row r="2" spans="1:12" ht="15.75">
       <c r="A2" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>0</v>
@@ -3694,16 +3152,16 @@
     </row>
     <row r="3" spans="1:12" ht="15.75">
       <c r="A3" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>0</v>
@@ -4135,7 +3593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L32"/>
   <sheetViews>
@@ -4199,16 +3657,16 @@
     </row>
     <row r="2" spans="1:12" ht="15.75">
       <c r="A2" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>0</v>
@@ -4231,16 +3689,16 @@
     </row>
     <row r="3" spans="1:12" ht="15.75">
       <c r="A3" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>0</v>
@@ -4672,7 +4130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L32"/>
   <sheetViews>
@@ -4736,16 +4194,16 @@
     </row>
     <row r="2" spans="1:12" ht="15.75">
       <c r="A2" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>0</v>
@@ -4768,16 +4226,16 @@
     </row>
     <row r="3" spans="1:12" ht="15.75">
       <c r="A3" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>0</v>
@@ -5207,509 +4665,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L31"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="53.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="49.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="52.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="96.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="5" width="80.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="5" width="90.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75">
-      <c r="A2" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="L2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="18" customFormat="1" ht="15.75">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3" s="19"/>
-      <c r="I3"/>
-      <c r="J3" s="19"/>
-      <c r="K3"/>
-      <c r="L3"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.75">
-      <c r="A4" s="8"/>
-      <c r="B4" s="11"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4" s="5"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.75">
-      <c r="A5" s="8"/>
-      <c r="B5" s="11"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5" s="5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.75">
-      <c r="A6" s="8"/>
-      <c r="B6" s="11"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6" s="5"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.75">
-      <c r="A7" s="8"/>
-      <c r="B7" s="11"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7" s="1"/>
-      <c r="F7"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="1"/>
-      <c r="L7"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="8"/>
-      <c r="B8" s="13"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8" s="7"/>
-      <c r="I8"/>
-      <c r="J8" s="4"/>
-      <c r="K8"/>
-      <c r="L8"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.75">
-      <c r="A9" s="8"/>
-      <c r="B9" s="11"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9" s="7"/>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-    </row>
-    <row r="10" spans="1:12" ht="16.5">
-      <c r="A10" s="8"/>
-      <c r="B10" s="11"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="8"/>
-      <c r="J10"/>
-      <c r="K10"/>
-      <c r="L10"/>
-    </row>
-    <row r="11" spans="1:12" ht="16.5">
-      <c r="A11" s="8"/>
-      <c r="B11" s="11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="8"/>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11"/>
-    </row>
-    <row r="12" spans="1:12" ht="16.5">
-      <c r="A12" s="8"/>
-      <c r="B12" s="11"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="8"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75">
-      <c r="A13" s="8"/>
-      <c r="B13" s="11"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13" s="7"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13"/>
-    </row>
-    <row r="14" spans="1:12" ht="16.5">
-      <c r="A14" s="8"/>
-      <c r="B14" s="11"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="8"/>
-      <c r="J14"/>
-      <c r="K14"/>
-      <c r="L14"/>
-    </row>
-    <row r="15" spans="1:12" ht="15.75">
-      <c r="A15" s="8"/>
-      <c r="B15" s="14"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.75">
-      <c r="A16" s="8"/>
-      <c r="B16" s="12"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.75">
-      <c r="A17" s="8"/>
-      <c r="B17" s="11"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17" s="1"/>
-      <c r="F17"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="1"/>
-      <c r="L17"/>
-    </row>
-    <row r="18" spans="1:12" ht="15.75">
-      <c r="A18" s="8"/>
-      <c r="B18" s="11"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18" s="1"/>
-      <c r="F18"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="1"/>
-      <c r="L18"/>
-    </row>
-    <row r="19" spans="1:12" ht="15.75">
-      <c r="A19" s="8"/>
-      <c r="B19" s="11"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19" s="1"/>
-      <c r="F19"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="1"/>
-      <c r="L19"/>
-    </row>
-    <row r="20" spans="1:12" s="9" customFormat="1" ht="15.75">
-      <c r="A20" s="8"/>
-      <c r="B20" s="15"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20" s="8"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20" s="10"/>
-      <c r="I20"/>
-      <c r="J20" s="13"/>
-      <c r="K20"/>
-      <c r="L20"/>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21" s="8"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21" s="4"/>
-      <c r="K21"/>
-      <c r="L21"/>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22" s="8"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22" s="4"/>
-      <c r="I22"/>
-      <c r="J22" s="4"/>
-      <c r="K22"/>
-      <c r="L22"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23" s="8"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
-      <c r="J23" s="4"/>
-      <c r="K23"/>
-      <c r="L23"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24" s="1"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
-      <c r="J24"/>
-      <c r="K24"/>
-      <c r="L24"/>
-    </row>
-    <row r="25" spans="1:12" ht="15.75">
-      <c r="A25"/>
-      <c r="B25" s="11"/>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="4"/>
-      <c r="K25"/>
-      <c r="L25"/>
-    </row>
-    <row r="26" spans="1:12" ht="15.75">
-      <c r="A26"/>
-      <c r="B26" s="11"/>
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="7"/>
-      <c r="K26"/>
-      <c r="L26"/>
-    </row>
-    <row r="27" spans="1:12" ht="15.75">
-      <c r="A27"/>
-      <c r="B27" s="11"/>
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27"/>
-      <c r="F27"/>
-      <c r="G27"/>
-      <c r="H27"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="4"/>
-      <c r="K27"/>
-      <c r="L27"/>
-    </row>
-    <row r="28" spans="1:12" ht="15.75">
-      <c r="A28"/>
-      <c r="B28" s="11"/>
-      <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28" s="1"/>
-      <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="4"/>
-      <c r="K28"/>
-      <c r="L28"/>
-    </row>
-    <row r="29" spans="1:12" ht="15.75">
-      <c r="A29"/>
-      <c r="B29" s="11"/>
-      <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29" s="1"/>
-      <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="4"/>
-      <c r="K29"/>
-      <c r="L29"/>
-    </row>
-    <row r="30" spans="1:12" ht="15.75">
-      <c r="A30"/>
-      <c r="B30" s="11"/>
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="G30"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="4"/>
-      <c r="K30"/>
-      <c r="L30"/>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="8"/>
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31" s="8"/>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="4"/>
-      <c r="K31"/>
-      <c r="L31"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding the new API's for IPA
</commit_message>
<xml_diff>
--- a/src/test/test-data/IPA.xlsx
+++ b/src/test/test-data/IPA.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1p-projects\1p-api-automation\src\test\test-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Competetitors" sheetId="1" r:id="rId1"/>
@@ -14,13 +19,15 @@
     <sheet name="Snapshot" sheetId="6" r:id="rId5"/>
     <sheet name="Techprofolio" sheetId="7" r:id="rId6"/>
     <sheet name="Techtrending" sheetId="8" r:id="rId7"/>
+    <sheet name="Countries" sheetId="10" r:id="rId8"/>
+    <sheet name="Comparision" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="84">
   <si>
     <t>GET</t>
   </si>
@@ -76,159 +83,210 @@
     <t>?query=laser&amp;querytype=technology</t>
   </si>
   <si>
+    <t>competitors - technology</t>
+  </si>
+  <si>
+    <t>API Test for the Competitors for the technology search</t>
+  </si>
+  <si>
+    <t>?query=laser&amp;querytype=company</t>
+  </si>
+  <si>
+    <t>competitors - company</t>
+  </si>
+  <si>
+    <t>dashboard-tech-profolio</t>
+  </si>
+  <si>
+    <t>API Test for the Dashboard for the technology search for chart type techprofolio</t>
+  </si>
+  <si>
+    <t>/analytics/dashboard</t>
+  </si>
+  <si>
+    <t>?query=Carbon&amp;querytype=technology&amp;charttype=techprofolio</t>
+  </si>
+  <si>
+    <t>dashboard-tech-trending</t>
+  </si>
+  <si>
+    <t>API Test for the Dashboard for the technology search for chart type trending</t>
+  </si>
+  <si>
+    <t>?query=Carbon&amp;querytype=technology&amp;charttype=techtrending</t>
+  </si>
+  <si>
+    <t>dashboard-tech-competitors</t>
+  </si>
+  <si>
+    <t>API Test for the Dashboard for the technology search for chart type competitors</t>
+  </si>
+  <si>
+    <t>?query=Carbon&amp;querytype=technology&amp;charttype=competitors</t>
+  </si>
+  <si>
+    <t>dashboard-company-profolio</t>
+  </si>
+  <si>
+    <t>API Test for the Dashboard for the company search for chart type techprofolio</t>
+  </si>
+  <si>
+    <t>?query=Carbon&amp;querytype=company&amp;charttype=techprofolio</t>
+  </si>
+  <si>
+    <t>dashboard-company-trending</t>
+  </si>
+  <si>
+    <t>API Test for the Dashboard for the company search for chart type trending</t>
+  </si>
+  <si>
+    <t>?query=Carbon&amp;querytype=company&amp;charttype=techtrending</t>
+  </si>
+  <si>
+    <t>dashboard-company-competitors</t>
+  </si>
+  <si>
+    <t>API Test for the Dashboard for the company search for chart type competitors</t>
+  </si>
+  <si>
+    <t>?query=Carbon&amp;querytype=company&amp;charttype=competitors</t>
+  </si>
+  <si>
+    <t>filters-technology</t>
+  </si>
+  <si>
+    <t>API Test for the Filter for the technology search</t>
+  </si>
+  <si>
+    <t>/analytics/filters</t>
+  </si>
+  <si>
+    <t>?query=Carbon&amp;querytype=technology</t>
+  </si>
+  <si>
+    <t>filters-company</t>
+  </si>
+  <si>
+    <t>API Test for the Filter for the company search</t>
+  </si>
+  <si>
+    <t>?query=Carbon&amp;querytype=company</t>
+  </si>
+  <si>
+    <t>resultset-technology</t>
+  </si>
+  <si>
+    <t>/analytics/resultset</t>
+  </si>
+  <si>
+    <t>resultset-company</t>
+  </si>
+  <si>
+    <t>snapshot-technology</t>
+  </si>
+  <si>
+    <t>API Test for snapshot for technology search</t>
+  </si>
+  <si>
+    <t>/analytics/snapshot</t>
+  </si>
+  <si>
+    <t>snapshot-company</t>
+  </si>
+  <si>
+    <t>API Test for snapshot for company search</t>
+  </si>
+  <si>
+    <t>techprofolio-technology</t>
+  </si>
+  <si>
+    <t>API Test for techprofolio for technology search</t>
+  </si>
+  <si>
+    <t>/analytics/techportfolio</t>
+  </si>
+  <si>
+    <t>techprofolio-company</t>
+  </si>
+  <si>
+    <t>API Test for techprofolio for company search</t>
+  </si>
+  <si>
+    <t>techtrending-technology</t>
+  </si>
+  <si>
+    <t>API Test for techtrending for technology search</t>
+  </si>
+  <si>
+    <t>/analytics/techtrending</t>
+  </si>
+  <si>
+    <t>techtrending-company</t>
+  </si>
+  <si>
+    <t>API Test for techtrending for company search</t>
+  </si>
+  <si>
+    <t>Countries-technology</t>
+  </si>
+  <si>
+    <t>/analytics/countries</t>
+  </si>
+  <si>
+    <t>?charttype=where&amp;query=JAVA&amp;querytype=technology</t>
+  </si>
+  <si>
+    <t>API Test for Countries for technology search</t>
+  </si>
+  <si>
+    <t>?charttype=where&amp;filter=grantStatus:U&amp;query=JAVA&amp;querytype=technology</t>
+  </si>
+  <si>
+    <t>?charttype=where&amp;filter=grantStatus:G&amp;query=JAVA&amp;querytype=technology</t>
+  </si>
+  <si>
+    <t>?charttype=where&amp;filter=grantStatus:A&amp;query=JAVA&amp;querytype=technology</t>
+  </si>
+  <si>
+    <t>?charttype=where&amp;filter=isBasic:B&amp;query=JAVA&amp;querytype=technology</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>competitors - technology</t>
-  </si>
-  <si>
-    <t>API Test for the Competitors for the technology search</t>
-  </si>
-  <si>
-    <t>?query=laser&amp;querytype=company</t>
-  </si>
-  <si>
-    <t>competitors - company</t>
-  </si>
-  <si>
-    <t>dashboard-tech-profolio</t>
-  </si>
-  <si>
-    <t>API Test for the Dashboard for the technology search for chart type techprofolio</t>
-  </si>
-  <si>
-    <t>/analytics/dashboard</t>
-  </si>
-  <si>
-    <t>?query=Carbon&amp;querytype=technology&amp;charttype=techprofolio</t>
-  </si>
-  <si>
-    <t>dashboard-tech-trending</t>
-  </si>
-  <si>
-    <t>API Test for the Dashboard for the technology search for chart type trending</t>
-  </si>
-  <si>
-    <t>?query=Carbon&amp;querytype=technology&amp;charttype=techtrending</t>
-  </si>
-  <si>
-    <t>dashboard-tech-competitors</t>
-  </si>
-  <si>
-    <t>API Test for the Dashboard for the technology search for chart type competitors</t>
-  </si>
-  <si>
-    <t>?query=Carbon&amp;querytype=technology&amp;charttype=competitors</t>
-  </si>
-  <si>
-    <t>dashboard-company-profolio</t>
-  </si>
-  <si>
-    <t>API Test for the Dashboard for the company search for chart type techprofolio</t>
-  </si>
-  <si>
-    <t>?query=Carbon&amp;querytype=company&amp;charttype=techprofolio</t>
-  </si>
-  <si>
-    <t>dashboard-company-trending</t>
-  </si>
-  <si>
-    <t>API Test for the Dashboard for the company search for chart type trending</t>
-  </si>
-  <si>
-    <t>?query=Carbon&amp;querytype=company&amp;charttype=techtrending</t>
-  </si>
-  <si>
-    <t>dashboard-company-competitors</t>
-  </si>
-  <si>
-    <t>API Test for the Dashboard for the company search for chart type competitors</t>
-  </si>
-  <si>
-    <t>?query=Carbon&amp;querytype=company&amp;charttype=competitors</t>
-  </si>
-  <si>
-    <t>filters-technology</t>
-  </si>
-  <si>
-    <t>API Test for the Filter for the technology search</t>
-  </si>
-  <si>
-    <t>/analytics/filters</t>
-  </si>
-  <si>
-    <t>?query=Carbon&amp;querytype=technology</t>
-  </si>
-  <si>
-    <t>filters-company</t>
-  </si>
-  <si>
-    <t>API Test for the Filter for the company search</t>
-  </si>
-  <si>
-    <t>?query=Carbon&amp;querytype=company</t>
-  </si>
-  <si>
-    <t>resultset-technology</t>
-  </si>
-  <si>
-    <t>/analytics/resultset</t>
-  </si>
-  <si>
-    <t>resultset-company</t>
-  </si>
-  <si>
-    <t>snapshot-technology</t>
-  </si>
-  <si>
-    <t>API Test for snapshot for technology search</t>
-  </si>
-  <si>
-    <t>/analytics/snapshot</t>
-  </si>
-  <si>
-    <t>snapshot-company</t>
-  </si>
-  <si>
-    <t>API Test for snapshot for company search</t>
-  </si>
-  <si>
-    <t>techprofolio-technology</t>
-  </si>
-  <si>
-    <t>API Test for techprofolio for technology search</t>
-  </si>
-  <si>
-    <t>/analytics/techportfolio</t>
-  </si>
-  <si>
-    <t>techprofolio-company</t>
-  </si>
-  <si>
-    <t>API Test for techprofolio for company search</t>
-  </si>
-  <si>
-    <t>techtrending-technology</t>
-  </si>
-  <si>
-    <t>API Test for techtrending for technology search</t>
-  </si>
-  <si>
-    <t>/analytics/techtrending</t>
-  </si>
-  <si>
-    <t>techtrending-company</t>
-  </si>
-  <si>
-    <t>API Test for techtrending for company search</t>
+    <t>Comparision-company</t>
+  </si>
+  <si>
+    <t>API Test for Comparision for Company search</t>
+  </si>
+  <si>
+    <t>/analytics/comparison</t>
+  </si>
+  <si>
+    <t>?charttype=comparison&amp;query=C1790_APPLE%23%23APPLE+INC&amp;querytype=company</t>
+  </si>
+  <si>
+    <t>?charttype=comparison&amp;filter=isBasic:B&amp;query=C1790_APPLE%23%23APPLE+INC&amp;querytype=company</t>
+  </si>
+  <si>
+    <t>?charttype=comparison&amp;filter=grantStatus:A&amp;query=C1790_APPLE%23%23APPLE+INC&amp;querytype=company</t>
+  </si>
+  <si>
+    <t>?charttype=comparison&amp;filter=grantStatus:G&amp;query=C1790_APPLE%23%23APPLE+INC&amp;querytype=company</t>
+  </si>
+  <si>
+    <t>?charttype=comparison&amp;filter=grantStatus:U&amp;query=C1790_APPLE%23%23APPLE+INC&amp;querytype=company</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -375,12 +433,41 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -427,7 +514,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -459,9 +546,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -493,6 +581,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -668,14 +757,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="5" width="53.140625" collapsed="true"/>
@@ -691,7 +780,7 @@
     <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -729,12 +818,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>20</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>13</v>
@@ -758,15 +847,15 @@
       </c>
       <c r="K2" s="1"/>
       <c r="L2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>13</v>
@@ -781,7 +870,7 @@
         <v>16</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
@@ -790,10 +879,10 @@
       </c>
       <c r="K3" s="1"/>
       <c r="L3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15.75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="11"/>
       <c r="C4"/>
@@ -807,7 +896,7 @@
       <c r="K4" s="1"/>
       <c r="L4"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="11"/>
       <c r="C5"/>
@@ -821,7 +910,7 @@
       <c r="K5" s="1"/>
       <c r="L5"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="11"/>
       <c r="C6"/>
@@ -835,7 +924,7 @@
       <c r="K6" s="1"/>
       <c r="L6"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="11"/>
       <c r="C7"/>
@@ -849,7 +938,7 @@
       <c r="K7"/>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="11"/>
       <c r="C8"/>
@@ -863,7 +952,7 @@
       <c r="K8"/>
       <c r="L8"/>
     </row>
-    <row r="9" spans="1:12" s="18" customFormat="1" ht="15.75">
+    <row r="9" spans="1:12" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="17"/>
       <c r="C9"/>
@@ -877,7 +966,7 @@
       <c r="K9"/>
       <c r="L9"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="11"/>
       <c r="C10"/>
@@ -891,7 +980,7 @@
       <c r="K10"/>
       <c r="L10"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="11"/>
       <c r="C11"/>
@@ -905,7 +994,7 @@
       <c r="K11"/>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75">
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="11"/>
       <c r="C12"/>
@@ -919,7 +1008,7 @@
       <c r="K12"/>
       <c r="L12"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75">
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="11"/>
       <c r="C13"/>
@@ -933,7 +1022,7 @@
       <c r="K13" s="1"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="13"/>
       <c r="C14"/>
@@ -947,7 +1036,7 @@
       <c r="K14"/>
       <c r="L14"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="11"/>
       <c r="C15"/>
@@ -961,7 +1050,7 @@
       <c r="K15"/>
       <c r="L15"/>
     </row>
-    <row r="16" spans="1:12" ht="16.5">
+    <row r="16" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="11"/>
       <c r="C16"/>
@@ -975,7 +1064,7 @@
       <c r="K16"/>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:12" ht="16.5">
+    <row r="17" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="11"/>
       <c r="C17"/>
@@ -989,7 +1078,7 @@
       <c r="K17"/>
       <c r="L17"/>
     </row>
-    <row r="18" spans="1:12" ht="16.5">
+    <row r="18" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="11"/>
       <c r="C18"/>
@@ -1003,7 +1092,7 @@
       <c r="K18"/>
       <c r="L18"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75">
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="11"/>
       <c r="C19"/>
@@ -1017,7 +1106,7 @@
       <c r="K19"/>
       <c r="L19"/>
     </row>
-    <row r="20" spans="1:12" ht="16.5">
+    <row r="20" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="11"/>
       <c r="C20"/>
@@ -1031,7 +1120,7 @@
       <c r="K20"/>
       <c r="L20"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75">
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="14"/>
       <c r="C21"/>
@@ -1045,7 +1134,7 @@
       <c r="K21"/>
       <c r="L21"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75">
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="12"/>
       <c r="C22"/>
@@ -1059,7 +1148,7 @@
       <c r="K22"/>
       <c r="L22"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75">
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="11"/>
       <c r="C23"/>
@@ -1073,7 +1162,7 @@
       <c r="K23" s="1"/>
       <c r="L23"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75">
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="11"/>
       <c r="C24"/>
@@ -1087,7 +1176,7 @@
       <c r="K24" s="1"/>
       <c r="L24"/>
     </row>
-    <row r="25" spans="1:12" ht="15.75">
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="11"/>
       <c r="C25"/>
@@ -1101,7 +1190,7 @@
       <c r="K25" s="1"/>
       <c r="L25"/>
     </row>
-    <row r="26" spans="1:12" s="9" customFormat="1" ht="15.75">
+    <row r="26" spans="1:12" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="15"/>
       <c r="C26"/>
@@ -1115,7 +1204,7 @@
       <c r="K26"/>
       <c r="L26"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -1129,7 +1218,7 @@
       <c r="K27"/>
       <c r="L27"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -1143,7 +1232,7 @@
       <c r="K28"/>
       <c r="L28"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -1157,7 +1246,7 @@
       <c r="K29"/>
       <c r="L29"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -1171,7 +1260,7 @@
       <c r="K30"/>
       <c r="L30"/>
     </row>
-    <row r="31" spans="1:12" ht="15.75">
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31" s="11"/>
       <c r="C31"/>
@@ -1185,7 +1274,7 @@
       <c r="K31"/>
       <c r="L31"/>
     </row>
-    <row r="32" spans="1:12" ht="15.75">
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32" s="11"/>
       <c r="C32"/>
@@ -1199,7 +1288,7 @@
       <c r="K32"/>
       <c r="L32"/>
     </row>
-    <row r="33" spans="1:10" ht="15.75">
+    <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33"/>
       <c r="B33" s="11"/>
       <c r="C33"/>
@@ -1213,7 +1302,7 @@
       <c r="K33"/>
       <c r="L33"/>
     </row>
-    <row r="34" spans="1:10" ht="15.75">
+    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34"/>
       <c r="B34" s="11"/>
       <c r="C34"/>
@@ -1227,7 +1316,7 @@
       <c r="K34"/>
       <c r="L34"/>
     </row>
-    <row r="35" spans="1:10" ht="15.75">
+    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35"/>
       <c r="B35" s="11"/>
       <c r="C35"/>
@@ -1241,7 +1330,7 @@
       <c r="K35"/>
       <c r="L35"/>
     </row>
-    <row r="36" spans="1:10" ht="15.75">
+    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36"/>
       <c r="B36" s="11"/>
       <c r="C36"/>
@@ -1255,7 +1344,7 @@
       <c r="K36"/>
       <c r="L36"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37"/>
       <c r="C37"/>
@@ -1276,14 +1365,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="5" width="53.140625" collapsed="true"/>
@@ -1299,7 +1388,7 @@
     <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1337,18 +1426,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="31.5">
+    <row r="2" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>24</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>0</v>
@@ -1357,7 +1446,7 @@
         <v>16</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
@@ -1366,21 +1455,21 @@
       </c>
       <c r="K2" s="1"/>
       <c r="L2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="31.5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>28</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>0</v>
@@ -1389,7 +1478,7 @@
         <v>16</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
@@ -1398,21 +1487,21 @@
       </c>
       <c r="K3" s="1"/>
       <c r="L3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="31.5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>31</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>0</v>
@@ -1421,7 +1510,7 @@
         <v>16</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
@@ -1430,21 +1519,21 @@
       </c>
       <c r="K4" s="1"/>
       <c r="L4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="31.5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>33</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>34</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>0</v>
@@ -1453,7 +1542,7 @@
         <v>16</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="1"/>
@@ -1462,21 +1551,21 @@
       </c>
       <c r="K5" s="1"/>
       <c r="L5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="31.5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>37</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>0</v>
@@ -1485,7 +1574,7 @@
         <v>16</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="1"/>
@@ -1494,21 +1583,21 @@
       </c>
       <c r="K6" s="1"/>
       <c r="L6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="31.5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>40</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>0</v>
@@ -1517,7 +1606,7 @@
         <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H7"/>
       <c r="I7"/>
@@ -1526,10 +1615,10 @@
       </c>
       <c r="K7"/>
       <c r="L7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="11"/>
       <c r="C8"/>
@@ -1543,7 +1632,7 @@
       <c r="K8"/>
       <c r="L8"/>
     </row>
-    <row r="9" spans="1:12" s="18" customFormat="1" ht="15.75">
+    <row r="9" spans="1:12" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="17"/>
       <c r="C9"/>
@@ -1557,7 +1646,7 @@
       <c r="K9"/>
       <c r="L9"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="11"/>
       <c r="C10"/>
@@ -1571,7 +1660,7 @@
       <c r="K10"/>
       <c r="L10"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="11"/>
       <c r="C11"/>
@@ -1585,7 +1674,7 @@
       <c r="K11"/>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75">
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="11"/>
       <c r="C12"/>
@@ -1599,7 +1688,7 @@
       <c r="K12"/>
       <c r="L12"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75">
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="11"/>
       <c r="C13"/>
@@ -1613,7 +1702,7 @@
       <c r="K13" s="1"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="13"/>
       <c r="C14"/>
@@ -1627,7 +1716,7 @@
       <c r="K14"/>
       <c r="L14"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="11"/>
       <c r="C15"/>
@@ -1641,7 +1730,7 @@
       <c r="K15"/>
       <c r="L15"/>
     </row>
-    <row r="16" spans="1:12" ht="16.5">
+    <row r="16" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="11"/>
       <c r="C16"/>
@@ -1655,7 +1744,7 @@
       <c r="K16"/>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:12" ht="16.5">
+    <row r="17" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="11"/>
       <c r="C17"/>
@@ -1669,7 +1758,7 @@
       <c r="K17"/>
       <c r="L17"/>
     </row>
-    <row r="18" spans="1:12" ht="16.5">
+    <row r="18" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="11"/>
       <c r="C18"/>
@@ -1683,7 +1772,7 @@
       <c r="K18"/>
       <c r="L18"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75">
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="11"/>
       <c r="C19"/>
@@ -1697,7 +1786,7 @@
       <c r="K19"/>
       <c r="L19"/>
     </row>
-    <row r="20" spans="1:12" ht="16.5">
+    <row r="20" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="11"/>
       <c r="C20"/>
@@ -1711,7 +1800,7 @@
       <c r="K20"/>
       <c r="L20"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75">
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="14"/>
       <c r="C21"/>
@@ -1725,7 +1814,7 @@
       <c r="K21"/>
       <c r="L21"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75">
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="12"/>
       <c r="C22"/>
@@ -1739,7 +1828,7 @@
       <c r="K22"/>
       <c r="L22"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75">
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="11"/>
       <c r="C23"/>
@@ -1753,7 +1842,7 @@
       <c r="K23" s="1"/>
       <c r="L23"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75">
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="11"/>
       <c r="C24"/>
@@ -1767,7 +1856,7 @@
       <c r="K24" s="1"/>
       <c r="L24"/>
     </row>
-    <row r="25" spans="1:12" ht="15.75">
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="11"/>
       <c r="C25"/>
@@ -1781,7 +1870,7 @@
       <c r="K25" s="1"/>
       <c r="L25"/>
     </row>
-    <row r="26" spans="1:12" s="9" customFormat="1" ht="15.75">
+    <row r="26" spans="1:12" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="15"/>
       <c r="C26"/>
@@ -1795,7 +1884,7 @@
       <c r="K26"/>
       <c r="L26"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -1809,7 +1898,7 @@
       <c r="K27"/>
       <c r="L27"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -1823,7 +1912,7 @@
       <c r="K28"/>
       <c r="L28"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -1837,7 +1926,7 @@
       <c r="K29"/>
       <c r="L29"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -1851,7 +1940,7 @@
       <c r="K30"/>
       <c r="L30"/>
     </row>
-    <row r="31" spans="1:12" ht="15.75">
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31" s="11"/>
       <c r="C31"/>
@@ -1865,7 +1954,7 @@
       <c r="K31"/>
       <c r="L31"/>
     </row>
-    <row r="32" spans="1:12" ht="15.75">
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32" s="11"/>
       <c r="C32"/>
@@ -1879,7 +1968,7 @@
       <c r="K32"/>
       <c r="L32"/>
     </row>
-    <row r="33" spans="1:10" ht="15.75">
+    <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33"/>
       <c r="B33" s="11"/>
       <c r="C33"/>
@@ -1893,7 +1982,7 @@
       <c r="K33"/>
       <c r="L33"/>
     </row>
-    <row r="34" spans="1:10" ht="15.75">
+    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34"/>
       <c r="B34" s="11"/>
       <c r="C34"/>
@@ -1907,7 +1996,7 @@
       <c r="K34"/>
       <c r="L34"/>
     </row>
-    <row r="35" spans="1:10" ht="15.75">
+    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35"/>
       <c r="B35" s="11"/>
       <c r="C35"/>
@@ -1921,7 +2010,7 @@
       <c r="K35"/>
       <c r="L35"/>
     </row>
-    <row r="36" spans="1:10" ht="15.75">
+    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36"/>
       <c r="B36" s="11"/>
       <c r="C36"/>
@@ -1935,7 +2024,7 @@
       <c r="K36"/>
       <c r="L36"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37"/>
       <c r="C37"/>
@@ -1955,14 +2044,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="5" width="53.140625" collapsed="true"/>
@@ -1978,7 +2067,7 @@
     <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2016,18 +2105,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>0</v>
@@ -2036,7 +2125,7 @@
         <v>16</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
@@ -2045,21 +2134,21 @@
       </c>
       <c r="K2" s="1"/>
       <c r="L2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>46</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>0</v>
@@ -2068,7 +2157,7 @@
         <v>16</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
@@ -2077,10 +2166,10 @@
       </c>
       <c r="K3" s="1"/>
       <c r="L3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15.75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="11"/>
       <c r="C4"/>
@@ -2094,7 +2183,7 @@
       <c r="K4"/>
       <c r="L4"/>
     </row>
-    <row r="5" spans="1:12" s="18" customFormat="1" ht="15.75">
+    <row r="5" spans="1:12" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
       <c r="C5"/>
@@ -2108,7 +2197,7 @@
       <c r="K5"/>
       <c r="L5"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="11"/>
       <c r="C6"/>
@@ -2122,7 +2211,7 @@
       <c r="K6"/>
       <c r="L6"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="11"/>
       <c r="C7"/>
@@ -2136,7 +2225,7 @@
       <c r="K7"/>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="11"/>
       <c r="C8"/>
@@ -2150,7 +2239,7 @@
       <c r="K8"/>
       <c r="L8"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="11"/>
       <c r="C9"/>
@@ -2164,7 +2253,7 @@
       <c r="K9" s="1"/>
       <c r="L9"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="13"/>
       <c r="C10"/>
@@ -2178,7 +2267,7 @@
       <c r="K10"/>
       <c r="L10"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="11"/>
       <c r="C11"/>
@@ -2192,7 +2281,7 @@
       <c r="K11"/>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:12" ht="16.5">
+    <row r="12" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="11"/>
       <c r="C12"/>
@@ -2206,7 +2295,7 @@
       <c r="K12"/>
       <c r="L12"/>
     </row>
-    <row r="13" spans="1:12" ht="16.5">
+    <row r="13" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="11"/>
       <c r="C13"/>
@@ -2220,7 +2309,7 @@
       <c r="K13"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:12" ht="16.5">
+    <row r="14" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="11"/>
       <c r="C14"/>
@@ -2234,7 +2323,7 @@
       <c r="K14"/>
       <c r="L14"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="11"/>
       <c r="C15"/>
@@ -2248,7 +2337,7 @@
       <c r="K15"/>
       <c r="L15"/>
     </row>
-    <row r="16" spans="1:12" ht="16.5">
+    <row r="16" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="11"/>
       <c r="C16"/>
@@ -2262,7 +2351,7 @@
       <c r="K16"/>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75">
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="14"/>
       <c r="C17"/>
@@ -2276,7 +2365,7 @@
       <c r="K17"/>
       <c r="L17"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75">
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="12"/>
       <c r="C18"/>
@@ -2290,7 +2379,7 @@
       <c r="K18"/>
       <c r="L18"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75">
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="11"/>
       <c r="C19"/>
@@ -2304,7 +2393,7 @@
       <c r="K19" s="1"/>
       <c r="L19"/>
     </row>
-    <row r="20" spans="1:12" ht="15.75">
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="11"/>
       <c r="C20"/>
@@ -2318,7 +2407,7 @@
       <c r="K20" s="1"/>
       <c r="L20"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75">
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="11"/>
       <c r="C21"/>
@@ -2332,7 +2421,7 @@
       <c r="K21" s="1"/>
       <c r="L21"/>
     </row>
-    <row r="22" spans="1:12" s="9" customFormat="1" ht="15.75">
+    <row r="22" spans="1:12" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="15"/>
       <c r="C22"/>
@@ -2346,7 +2435,7 @@
       <c r="K22"/>
       <c r="L22"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -2360,7 +2449,7 @@
       <c r="K23"/>
       <c r="L23"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -2374,7 +2463,7 @@
       <c r="K24"/>
       <c r="L24"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -2388,7 +2477,7 @@
       <c r="K25"/>
       <c r="L25"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -2402,7 +2491,7 @@
       <c r="K26"/>
       <c r="L26"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75">
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27" s="11"/>
       <c r="C27"/>
@@ -2416,7 +2505,7 @@
       <c r="K27"/>
       <c r="L27"/>
     </row>
-    <row r="28" spans="1:12" ht="15.75">
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="B28" s="11"/>
       <c r="C28"/>
@@ -2430,7 +2519,7 @@
       <c r="K28"/>
       <c r="L28"/>
     </row>
-    <row r="29" spans="1:12" ht="15.75">
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29" s="11"/>
       <c r="C29"/>
@@ -2444,7 +2533,7 @@
       <c r="K29"/>
       <c r="L29"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75">
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30" s="11"/>
       <c r="C30"/>
@@ -2458,7 +2547,7 @@
       <c r="K30"/>
       <c r="L30"/>
     </row>
-    <row r="31" spans="1:12" ht="15.75">
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31" s="11"/>
       <c r="C31"/>
@@ -2472,7 +2561,7 @@
       <c r="K31"/>
       <c r="L31"/>
     </row>
-    <row r="32" spans="1:12" ht="15.75">
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32" s="11"/>
       <c r="C32"/>
@@ -2486,7 +2575,7 @@
       <c r="K32"/>
       <c r="L32"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33"/>
       <c r="C33"/>
@@ -2506,14 +2595,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="5" width="53.140625" collapsed="true"/>
@@ -2529,7 +2618,7 @@
     <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2567,18 +2656,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>0</v>
@@ -2587,7 +2676,7 @@
         <v>16</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
@@ -2596,21 +2685,21 @@
       </c>
       <c r="K2" s="1"/>
       <c r="L2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>0</v>
@@ -2619,7 +2708,7 @@
         <v>16</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
@@ -2628,10 +2717,10 @@
       </c>
       <c r="K3" s="1"/>
       <c r="L3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15.75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="11"/>
       <c r="C4"/>
@@ -2645,7 +2734,7 @@
       <c r="K4"/>
       <c r="L4"/>
     </row>
-    <row r="5" spans="1:12" s="18" customFormat="1" ht="15.75">
+    <row r="5" spans="1:12" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
       <c r="C5"/>
@@ -2659,7 +2748,7 @@
       <c r="K5"/>
       <c r="L5"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="11"/>
       <c r="C6"/>
@@ -2673,7 +2762,7 @@
       <c r="K6"/>
       <c r="L6"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="11"/>
       <c r="C7"/>
@@ -2687,7 +2776,7 @@
       <c r="K7"/>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="11"/>
       <c r="C8"/>
@@ -2701,7 +2790,7 @@
       <c r="K8"/>
       <c r="L8"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="11"/>
       <c r="C9"/>
@@ -2715,7 +2804,7 @@
       <c r="K9" s="1"/>
       <c r="L9"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="13"/>
       <c r="C10"/>
@@ -2729,7 +2818,7 @@
       <c r="K10"/>
       <c r="L10"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="11"/>
       <c r="C11"/>
@@ -2743,7 +2832,7 @@
       <c r="K11"/>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:12" ht="16.5">
+    <row r="12" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="11"/>
       <c r="C12"/>
@@ -2757,7 +2846,7 @@
       <c r="K12"/>
       <c r="L12"/>
     </row>
-    <row r="13" spans="1:12" ht="16.5">
+    <row r="13" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="11"/>
       <c r="C13"/>
@@ -2771,7 +2860,7 @@
       <c r="K13"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:12" ht="16.5">
+    <row r="14" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="11"/>
       <c r="C14"/>
@@ -2785,7 +2874,7 @@
       <c r="K14"/>
       <c r="L14"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="11"/>
       <c r="C15"/>
@@ -2799,7 +2888,7 @@
       <c r="K15"/>
       <c r="L15"/>
     </row>
-    <row r="16" spans="1:12" ht="16.5">
+    <row r="16" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="11"/>
       <c r="C16"/>
@@ -2813,7 +2902,7 @@
       <c r="K16"/>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75">
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="14"/>
       <c r="C17"/>
@@ -2827,7 +2916,7 @@
       <c r="K17"/>
       <c r="L17"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75">
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="12"/>
       <c r="C18"/>
@@ -2841,7 +2930,7 @@
       <c r="K18"/>
       <c r="L18"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75">
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="11"/>
       <c r="C19"/>
@@ -2855,7 +2944,7 @@
       <c r="K19" s="1"/>
       <c r="L19"/>
     </row>
-    <row r="20" spans="1:12" ht="15.75">
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="11"/>
       <c r="C20"/>
@@ -2869,7 +2958,7 @@
       <c r="K20" s="1"/>
       <c r="L20"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75">
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="11"/>
       <c r="C21"/>
@@ -2883,7 +2972,7 @@
       <c r="K21" s="1"/>
       <c r="L21"/>
     </row>
-    <row r="22" spans="1:12" s="9" customFormat="1" ht="15.75">
+    <row r="22" spans="1:12" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="15"/>
       <c r="C22"/>
@@ -2897,7 +2986,7 @@
       <c r="K22"/>
       <c r="L22"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -2911,7 +3000,7 @@
       <c r="K23"/>
       <c r="L23"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -2925,7 +3014,7 @@
       <c r="K24"/>
       <c r="L24"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -2939,7 +3028,7 @@
       <c r="K25"/>
       <c r="L25"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -2953,7 +3042,7 @@
       <c r="K26"/>
       <c r="L26"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75">
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27" s="11"/>
       <c r="C27"/>
@@ -2967,7 +3056,7 @@
       <c r="K27"/>
       <c r="L27"/>
     </row>
-    <row r="28" spans="1:12" ht="15.75">
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="B28" s="11"/>
       <c r="C28"/>
@@ -2981,7 +3070,7 @@
       <c r="K28"/>
       <c r="L28"/>
     </row>
-    <row r="29" spans="1:12" ht="15.75">
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29" s="11"/>
       <c r="C29"/>
@@ -2995,7 +3084,7 @@
       <c r="K29"/>
       <c r="L29"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75">
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30" s="11"/>
       <c r="C30"/>
@@ -3009,7 +3098,7 @@
       <c r="K30"/>
       <c r="L30"/>
     </row>
-    <row r="31" spans="1:12" ht="15.75">
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31" s="11"/>
       <c r="C31"/>
@@ -3023,7 +3112,7 @@
       <c r="K31"/>
       <c r="L31"/>
     </row>
-    <row r="32" spans="1:12" ht="15.75">
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32" s="11"/>
       <c r="C32"/>
@@ -3037,7 +3126,7 @@
       <c r="K32"/>
       <c r="L32"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33"/>
       <c r="C33"/>
@@ -3057,14 +3146,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="5" width="53.140625" collapsed="true"/>
@@ -3080,7 +3169,7 @@
     <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -3118,18 +3207,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>52</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>53</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>0</v>
@@ -3138,7 +3227,7 @@
         <v>16</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
@@ -3147,21 +3236,21 @@
       </c>
       <c r="K2" s="1"/>
       <c r="L2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>55</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>56</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>0</v>
@@ -3170,7 +3259,7 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
@@ -3179,10 +3268,10 @@
       </c>
       <c r="K3"/>
       <c r="L3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="18" customFormat="1" ht="15.75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="17"/>
       <c r="C4"/>
@@ -3196,7 +3285,7 @@
       <c r="K4"/>
       <c r="L4"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="11"/>
       <c r="C5"/>
@@ -3210,7 +3299,7 @@
       <c r="K5"/>
       <c r="L5"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="11"/>
       <c r="C6"/>
@@ -3224,7 +3313,7 @@
       <c r="K6"/>
       <c r="L6"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="11"/>
       <c r="C7"/>
@@ -3238,7 +3327,7 @@
       <c r="K7"/>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="11"/>
       <c r="C8"/>
@@ -3252,7 +3341,7 @@
       <c r="K8" s="1"/>
       <c r="L8"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="13"/>
       <c r="C9"/>
@@ -3266,7 +3355,7 @@
       <c r="K9"/>
       <c r="L9"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="11"/>
       <c r="C10"/>
@@ -3280,7 +3369,7 @@
       <c r="K10"/>
       <c r="L10"/>
     </row>
-    <row r="11" spans="1:12" ht="16.5">
+    <row r="11" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="11"/>
       <c r="C11"/>
@@ -3294,7 +3383,7 @@
       <c r="K11"/>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:12" ht="16.5">
+    <row r="12" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="11"/>
       <c r="C12"/>
@@ -3308,7 +3397,7 @@
       <c r="K12"/>
       <c r="L12"/>
     </row>
-    <row r="13" spans="1:12" ht="16.5">
+    <row r="13" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="11"/>
       <c r="C13"/>
@@ -3322,7 +3411,7 @@
       <c r="K13"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="11"/>
       <c r="C14"/>
@@ -3336,7 +3425,7 @@
       <c r="K14"/>
       <c r="L14"/>
     </row>
-    <row r="15" spans="1:12" ht="16.5">
+    <row r="15" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="11"/>
       <c r="C15"/>
@@ -3350,7 +3439,7 @@
       <c r="K15"/>
       <c r="L15"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="14"/>
       <c r="C16"/>
@@ -3364,7 +3453,7 @@
       <c r="K16"/>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75">
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="12"/>
       <c r="C17"/>
@@ -3378,7 +3467,7 @@
       <c r="K17"/>
       <c r="L17"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75">
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="11"/>
       <c r="C18"/>
@@ -3392,7 +3481,7 @@
       <c r="K18" s="1"/>
       <c r="L18"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75">
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="11"/>
       <c r="C19"/>
@@ -3406,7 +3495,7 @@
       <c r="K19" s="1"/>
       <c r="L19"/>
     </row>
-    <row r="20" spans="1:12" ht="15.75">
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="11"/>
       <c r="C20"/>
@@ -3420,7 +3509,7 @@
       <c r="K20" s="1"/>
       <c r="L20"/>
     </row>
-    <row r="21" spans="1:12" s="9" customFormat="1" ht="15.75">
+    <row r="21" spans="1:12" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="15"/>
       <c r="C21"/>
@@ -3434,7 +3523,7 @@
       <c r="K21"/>
       <c r="L21"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -3448,7 +3537,7 @@
       <c r="K22"/>
       <c r="L22"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -3462,7 +3551,7 @@
       <c r="K23"/>
       <c r="L23"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -3476,7 +3565,7 @@
       <c r="K24"/>
       <c r="L24"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -3490,7 +3579,7 @@
       <c r="K25"/>
       <c r="L25"/>
     </row>
-    <row r="26" spans="1:12" ht="15.75">
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="B26" s="11"/>
       <c r="C26"/>
@@ -3504,7 +3593,7 @@
       <c r="K26"/>
       <c r="L26"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75">
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27" s="11"/>
       <c r="C27"/>
@@ -3518,7 +3607,7 @@
       <c r="K27"/>
       <c r="L27"/>
     </row>
-    <row r="28" spans="1:12" ht="15.75">
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="B28" s="11"/>
       <c r="C28"/>
@@ -3532,7 +3621,7 @@
       <c r="K28"/>
       <c r="L28"/>
     </row>
-    <row r="29" spans="1:12" ht="15.75">
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29" s="11"/>
       <c r="C29"/>
@@ -3546,7 +3635,7 @@
       <c r="K29"/>
       <c r="L29"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75">
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30" s="11"/>
       <c r="C30"/>
@@ -3560,7 +3649,7 @@
       <c r="K30"/>
       <c r="L30"/>
     </row>
-    <row r="31" spans="1:12" ht="15.75">
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31" s="11"/>
       <c r="C31"/>
@@ -3574,7 +3663,7 @@
       <c r="K31"/>
       <c r="L31"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32"/>
       <c r="C32"/>
@@ -3594,14 +3683,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="5" width="53.140625" collapsed="true"/>
@@ -3617,7 +3706,7 @@
     <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -3655,18 +3744,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>57</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>58</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>0</v>
@@ -3684,21 +3773,21 @@
       </c>
       <c r="K2" s="1"/>
       <c r="L2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>61</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>0</v>
@@ -3707,7 +3796,7 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
@@ -3716,10 +3805,10 @@
       </c>
       <c r="K3"/>
       <c r="L3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="18" customFormat="1" ht="15.75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="17"/>
       <c r="C4"/>
@@ -3733,7 +3822,7 @@
       <c r="K4"/>
       <c r="L4"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="11"/>
       <c r="C5"/>
@@ -3747,7 +3836,7 @@
       <c r="K5"/>
       <c r="L5"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="11"/>
       <c r="C6"/>
@@ -3761,7 +3850,7 @@
       <c r="K6"/>
       <c r="L6"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="11"/>
       <c r="C7"/>
@@ -3775,7 +3864,7 @@
       <c r="K7"/>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="11"/>
       <c r="C8"/>
@@ -3789,7 +3878,7 @@
       <c r="K8" s="1"/>
       <c r="L8"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="13"/>
       <c r="C9"/>
@@ -3803,7 +3892,7 @@
       <c r="K9"/>
       <c r="L9"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="11"/>
       <c r="C10"/>
@@ -3817,7 +3906,7 @@
       <c r="K10"/>
       <c r="L10"/>
     </row>
-    <row r="11" spans="1:12" ht="16.5">
+    <row r="11" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="11"/>
       <c r="C11"/>
@@ -3831,7 +3920,7 @@
       <c r="K11"/>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:12" ht="16.5">
+    <row r="12" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="11"/>
       <c r="C12"/>
@@ -3845,7 +3934,7 @@
       <c r="K12"/>
       <c r="L12"/>
     </row>
-    <row r="13" spans="1:12" ht="16.5">
+    <row r="13" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="11"/>
       <c r="C13"/>
@@ -3859,7 +3948,7 @@
       <c r="K13"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="11"/>
       <c r="C14"/>
@@ -3873,7 +3962,7 @@
       <c r="K14"/>
       <c r="L14"/>
     </row>
-    <row r="15" spans="1:12" ht="16.5">
+    <row r="15" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="11"/>
       <c r="C15"/>
@@ -3887,7 +3976,7 @@
       <c r="K15"/>
       <c r="L15"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="14"/>
       <c r="C16"/>
@@ -3901,7 +3990,7 @@
       <c r="K16"/>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75">
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="12"/>
       <c r="C17"/>
@@ -3915,7 +4004,7 @@
       <c r="K17"/>
       <c r="L17"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75">
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="11"/>
       <c r="C18"/>
@@ -3929,7 +4018,7 @@
       <c r="K18" s="1"/>
       <c r="L18"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75">
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="11"/>
       <c r="C19"/>
@@ -3943,7 +4032,7 @@
       <c r="K19" s="1"/>
       <c r="L19"/>
     </row>
-    <row r="20" spans="1:12" ht="15.75">
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="11"/>
       <c r="C20"/>
@@ -3957,7 +4046,7 @@
       <c r="K20" s="1"/>
       <c r="L20"/>
     </row>
-    <row r="21" spans="1:12" s="9" customFormat="1" ht="15.75">
+    <row r="21" spans="1:12" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="15"/>
       <c r="C21"/>
@@ -3971,7 +4060,7 @@
       <c r="K21"/>
       <c r="L21"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -3985,7 +4074,7 @@
       <c r="K22"/>
       <c r="L22"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -3999,7 +4088,7 @@
       <c r="K23"/>
       <c r="L23"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -4013,7 +4102,7 @@
       <c r="K24"/>
       <c r="L24"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -4027,7 +4116,7 @@
       <c r="K25"/>
       <c r="L25"/>
     </row>
-    <row r="26" spans="1:12" ht="15.75">
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="B26" s="11"/>
       <c r="C26"/>
@@ -4041,7 +4130,7 @@
       <c r="K26"/>
       <c r="L26"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75">
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27" s="11"/>
       <c r="C27"/>
@@ -4055,7 +4144,7 @@
       <c r="K27"/>
       <c r="L27"/>
     </row>
-    <row r="28" spans="1:12" ht="15.75">
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="B28" s="11"/>
       <c r="C28"/>
@@ -4069,7 +4158,7 @@
       <c r="K28"/>
       <c r="L28"/>
     </row>
-    <row r="29" spans="1:12" ht="15.75">
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29" s="11"/>
       <c r="C29"/>
@@ -4083,7 +4172,7 @@
       <c r="K29"/>
       <c r="L29"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75">
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30" s="11"/>
       <c r="C30"/>
@@ -4097,7 +4186,7 @@
       <c r="K30"/>
       <c r="L30"/>
     </row>
-    <row r="31" spans="1:12" ht="15.75">
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31" s="11"/>
       <c r="C31"/>
@@ -4111,7 +4200,7 @@
       <c r="K31"/>
       <c r="L31"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32"/>
       <c r="C32"/>
@@ -4131,14 +4220,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="5" width="53.140625" collapsed="true"/>
@@ -4154,7 +4243,7 @@
     <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -4192,18 +4281,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>62</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>63</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>0</v>
@@ -4221,21 +4310,21 @@
       </c>
       <c r="K2" s="1"/>
       <c r="L2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>66</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>0</v>
@@ -4244,7 +4333,7 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
@@ -4253,10 +4342,10 @@
       </c>
       <c r="K3"/>
       <c r="L3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="18" customFormat="1" ht="15.75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="17"/>
       <c r="C4"/>
@@ -4270,7 +4359,7 @@
       <c r="K4"/>
       <c r="L4"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="11"/>
       <c r="C5"/>
@@ -4284,7 +4373,7 @@
       <c r="K5"/>
       <c r="L5"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="11"/>
       <c r="C6"/>
@@ -4298,7 +4387,7 @@
       <c r="K6"/>
       <c r="L6"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="11"/>
       <c r="C7"/>
@@ -4312,7 +4401,7 @@
       <c r="K7"/>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="11"/>
       <c r="C8"/>
@@ -4326,7 +4415,7 @@
       <c r="K8" s="1"/>
       <c r="L8"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="13"/>
       <c r="C9"/>
@@ -4340,7 +4429,7 @@
       <c r="K9"/>
       <c r="L9"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="11"/>
       <c r="C10"/>
@@ -4354,7 +4443,7 @@
       <c r="K10"/>
       <c r="L10"/>
     </row>
-    <row r="11" spans="1:12" ht="16.5">
+    <row r="11" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="11"/>
       <c r="C11"/>
@@ -4368,7 +4457,7 @@
       <c r="K11"/>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:12" ht="16.5">
+    <row r="12" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="11"/>
       <c r="C12"/>
@@ -4382,7 +4471,7 @@
       <c r="K12"/>
       <c r="L12"/>
     </row>
-    <row r="13" spans="1:12" ht="16.5">
+    <row r="13" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="11"/>
       <c r="C13"/>
@@ -4396,7 +4485,7 @@
       <c r="K13"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="11"/>
       <c r="C14"/>
@@ -4410,7 +4499,7 @@
       <c r="K14"/>
       <c r="L14"/>
     </row>
-    <row r="15" spans="1:12" ht="16.5">
+    <row r="15" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="11"/>
       <c r="C15"/>
@@ -4424,7 +4513,7 @@
       <c r="K15"/>
       <c r="L15"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="14"/>
       <c r="C16"/>
@@ -4438,7 +4527,7 @@
       <c r="K16"/>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75">
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="12"/>
       <c r="C17"/>
@@ -4452,7 +4541,7 @@
       <c r="K17"/>
       <c r="L17"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75">
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="11"/>
       <c r="C18"/>
@@ -4466,7 +4555,7 @@
       <c r="K18" s="1"/>
       <c r="L18"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75">
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="11"/>
       <c r="C19"/>
@@ -4480,7 +4569,7 @@
       <c r="K19" s="1"/>
       <c r="L19"/>
     </row>
-    <row r="20" spans="1:12" ht="15.75">
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="11"/>
       <c r="C20"/>
@@ -4494,7 +4583,7 @@
       <c r="K20" s="1"/>
       <c r="L20"/>
     </row>
-    <row r="21" spans="1:12" s="9" customFormat="1" ht="15.75">
+    <row r="21" spans="1:12" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="15"/>
       <c r="C21"/>
@@ -4508,7 +4597,7 @@
       <c r="K21"/>
       <c r="L21"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -4522,7 +4611,7 @@
       <c r="K22"/>
       <c r="L22"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -4536,7 +4625,7 @@
       <c r="K23"/>
       <c r="L23"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -4550,7 +4639,7 @@
       <c r="K24"/>
       <c r="L24"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -4564,7 +4653,7 @@
       <c r="K25"/>
       <c r="L25"/>
     </row>
-    <row r="26" spans="1:12" ht="15.75">
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="B26" s="11"/>
       <c r="C26"/>
@@ -4578,7 +4667,7 @@
       <c r="K26"/>
       <c r="L26"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75">
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27" s="11"/>
       <c r="C27"/>
@@ -4592,7 +4681,7 @@
       <c r="K27"/>
       <c r="L27"/>
     </row>
-    <row r="28" spans="1:12" ht="15.75">
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="B28" s="11"/>
       <c r="C28"/>
@@ -4606,7 +4695,7 @@
       <c r="K28"/>
       <c r="L28"/>
     </row>
-    <row r="29" spans="1:12" ht="15.75">
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29" s="11"/>
       <c r="C29"/>
@@ -4620,7 +4709,7 @@
       <c r="K29"/>
       <c r="L29"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75">
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30" s="11"/>
       <c r="C30"/>
@@ -4634,7 +4723,7 @@
       <c r="K30"/>
       <c r="L30"/>
     </row>
-    <row r="31" spans="1:12" ht="15.75">
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31" s="11"/>
       <c r="C31"/>
@@ -4648,7 +4737,7 @@
       <c r="K31"/>
       <c r="L31"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32"/>
       <c r="C32"/>
@@ -4665,4 +4754,677 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection sqref="A1:L6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" style="5" width="24.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="40.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="22.28515625" collapsed="true"/>
+    <col min="5" max="5" style="5" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="5" width="22.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="5" width="34.7109375" collapsed="true"/>
+    <col min="8" max="8" style="5" width="9.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="5" width="11.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="12.0" collapsed="true"/>
+    <col min="11" max="16384" style="5" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="23"/>
+      <c r="L2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="27"/>
+      <c r="L3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="27"/>
+      <c r="L4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="27"/>
+      <c r="L5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="27"/>
+      <c r="L6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="42.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.42578125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="23"/>
+      <c r="L2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="27"/>
+      <c r="L3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="27"/>
+      <c r="L4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="27"/>
+      <c r="L5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="27"/>
+      <c r="L6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding new API's for IPA
</commit_message>
<xml_diff>
--- a/src/test/test-data/IPA.xlsx
+++ b/src/test/test-data/IPA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
   <sheets>
     <sheet name="Competetitors" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,14 @@
     <sheet name="Techtrending" sheetId="8" r:id="rId7"/>
     <sheet name="Countries" sheetId="10" r:id="rId8"/>
     <sheet name="Comparision" sheetId="11" r:id="rId9"/>
+    <sheet name="publicationDateStats" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="125725" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="90">
   <si>
     <t>GET</t>
   </si>
@@ -276,6 +277,24 @@
   </si>
   <si>
     <t>?charttype=comparison&amp;filter=grantStatus:U&amp;query=C1790_APPLE%23%23APPLE+INC&amp;querytype=company</t>
+  </si>
+  <si>
+    <t>publicationDateStats-Technology</t>
+  </si>
+  <si>
+    <t>API Test for publicationDateStats for Technology search</t>
+  </si>
+  <si>
+    <t>/analytics/publicationDateStats</t>
+  </si>
+  <si>
+    <t>publicationDateStats-Company</t>
+  </si>
+  <si>
+    <t>?filter=publicationYear:1..2017&amp;query=JAVA&amp;querytype=technology</t>
+  </si>
+  <si>
+    <t>?filter=publicationYear:1..2017&amp;query=C1790_APPLE%23%23APPLE+INC&amp;querytype=company</t>
   </si>
   <si>
     <t/>
@@ -382,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -450,9 +469,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -760,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,6 +1377,132 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="52.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="23"/>
+      <c r="L2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="23"/>
+      <c r="L3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5211,8 +5353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection sqref="A1:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>